<commit_message>
create parts of graph data
</commit_message>
<xml_diff>
--- a/experience/DQN/DQN_nohoho.xlsx
+++ b/experience/DQN/DQN_nohoho.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wagahai/Documents/h28_soturon/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nohoho" sheetId="2" r:id="rId1"/>
     <sheet name="skelton-t" sheetId="3" r:id="rId2"/>
+    <sheet name="DQN_nohoho_chain" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +22,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -334,7 +330,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -344,11 +340,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C51"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="82" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="19.5"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -356,42 +354,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -399,47 +397,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -447,27 +445,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -475,12 +473,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -488,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -496,42 +494,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>6</v>
       </c>
@@ -539,22 +537,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -562,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -570,17 +568,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -588,22 +586,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -611,12 +609,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -627,12 +625,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>1</v>
       </c>
@@ -640,6 +638,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -647,14 +646,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="19.5"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1">
         <v>1</v>
       </c>
@@ -693,6 +692,44 @@
       </c>
       <c r="M1">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>